<commit_message>
Added exception-thrown assertions to Members, Projects and Roles tests. Added ChangeWithWrongId and ChangeNonExisting in Roles repository test
</commit_message>
<xml_diff>
--- a/TimeKeeper.Test/TestDatabase/TimeKeeperTest.xlsx
+++ b/TimeKeeper.Test/TestDatabase/TimeKeeperTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TimeKeeper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TimeKeeper\TimeKeeper.Test\TestDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594B2866-6F09-4F5F-838E-1F351C405867}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CD0926-5C9E-41A7-AF6D-80600720249E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="1" r:id="rId1"/>
@@ -3379,7 +3379,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -3445,11 +3445,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet4" filterMode="1"/>
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:XFD99"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3475,7 +3475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>102</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>118</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>106</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>108</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>116</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>120</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>114</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>111</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>112</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>123</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>105</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>117</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>103</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>104</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>121</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>107</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>115</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>110</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>85</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>61</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>72</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>75</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>62</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>62</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>79</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>62</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>62</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>62</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>61</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>62</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>80</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>68</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>62</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>62</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>62</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>76</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>86</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>62</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>84</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>82</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>33</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>88</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>62</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>92</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>67</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>61</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>61</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>91</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>62</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>77</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>74</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>62</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>61</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>62</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>62</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>62</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>89</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>62</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>64</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>62</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>61</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>62</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>71</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>66</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>68</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>62</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>83</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>94</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>101</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>97</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>98</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>MATCH</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>99</v>
       </c>
@@ -5222,11 +5222,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E13173" xr:uid="{6BFDA35A-9284-4491-9FA2-2A115838ED89}">
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E13173" xr:uid="{6BFDA35A-9284-4491-9FA2-2A115838ED89}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>

</xml_diff>